<commit_message>
Add taxons and locus tests specification and implementations. Add some adjustments and bug fixes.
</commit_message>
<xml_diff>
--- a/docs/test cases/locus/LocusControllerTests.xlsx
+++ b/docs/test cases/locus/LocusControllerTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\Projeto\PhyloDB\docs\test cases\locus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976227A4-CBE4-4B37-A641-77A99CAB6143}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC02A9C-2583-47F0-B865-93E47429387D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="51">
   <si>
     <t>Parameter</t>
   </si>
@@ -78,33 +78,12 @@
     <t>Non-Existing</t>
   </si>
   <si>
-    <t>Existing, Non-Existing</t>
-  </si>
-  <si>
-    <t>Created</t>
-  </si>
-  <si>
-    <t>Updated</t>
-  </si>
-  <si>
-    <t>Existing with relations, Non-Existing</t>
-  </si>
-  <si>
-    <t>Deleted</t>
-  </si>
-  <si>
-    <t>Existing with relations</t>
-  </si>
-  <si>
     <t>outputmodel</t>
   </si>
   <si>
     <t>Error</t>
   </si>
   <si>
-    <t>p = some &gt;= 0</t>
-  </si>
-  <si>
     <t>Successful</t>
   </si>
   <si>
@@ -126,12 +105,6 @@
     <t>n = some &gt; 0</t>
   </si>
   <si>
-    <t>p = null, p = Empty, p = some &lt; 0</t>
-  </si>
-  <si>
-    <t>p &gt;= 0</t>
-  </si>
-  <si>
     <t>p &lt; 0</t>
   </si>
   <si>
@@ -144,37 +117,67 @@
     <t>inputModel</t>
   </si>
   <si>
-    <t>null, Object != inputModel</t>
-  </si>
-  <si>
     <t>204 No Content</t>
   </si>
   <si>
-    <t>String,  String != inputModel.key</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> String != inputModel.key</t>
-  </si>
-  <si>
     <t>401 Unauthorized</t>
   </si>
   <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -</t>
+  </si>
+  <si>
+    <t>null, with wrong fields</t>
+  </si>
+  <si>
+    <t>with wrong fields</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>true, false</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>400 Bad Request, 401 Unauthorized</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>Non-Existing, p &lt; 0</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>deleteProject</t>
+  </si>
+  <si>
     <t>getLoci</t>
   </si>
   <si>
+    <t>loci</t>
+  </si>
+  <si>
     <t>getLocus</t>
   </si>
   <si>
     <t>locus</t>
   </si>
   <si>
-    <t>locus_db</t>
-  </si>
-  <si>
     <t>saveLocus</t>
-  </si>
-  <si>
-    <t>deleteLocus</t>
   </si>
 </sst>
 </file>
@@ -206,7 +209,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -296,10 +299,19 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -307,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -321,8 +333,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -330,49 +360,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -381,9 +369,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -665,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -677,14 +676,12 @@
     <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -707,47 +704,47 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>33</v>
+      <c r="C4" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
-        <v>46</v>
+      <c r="A5" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
@@ -759,26 +756,26 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -793,13 +790,13 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="24"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="2" t="s">
         <v>9</v>
       </c>
@@ -807,15 +804,15 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -825,13 +822,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -841,13 +838,13 @@
         <v>2</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -856,14 +853,14 @@
       <c r="A14" s="3">
         <v>3</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>12</v>
+      <c r="B14" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -872,14 +869,14 @@
       <c r="A15" s="3">
         <v>4</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>12</v>
+      <c r="B15" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -889,96 +886,88 @@
         <v>5</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
-        <v>6</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>31</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
-        <v>7</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="A18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="A19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="A20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>2</v>
+      <c r="A21" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>36</v>
+      <c r="A22" s="13"/>
+      <c r="B22" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="19" t="s">
-        <v>47</v>
+      <c r="A23" s="21" t="s">
+        <v>49</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>4</v>
@@ -991,7 +980,7 @@
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="19"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="3" t="s">
         <v>5</v>
       </c>
@@ -1003,26 +992,26 @@
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="20" t="s">
-        <v>23</v>
+      <c r="A25" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="21"/>
+      <c r="A26" s="13"/>
       <c r="B26" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1037,502 +1026,465 @@
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="2" t="s">
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="18"/>
+      <c r="A29" s="14"/>
       <c r="B29" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="C29" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>1</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>2</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
+      <c r="E31" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="3" t="s">
+      <c r="A32" s="8">
+        <v>3</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="8">
         <v>4</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="B33" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>14</v>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="19"/>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="B37" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B38" s="13" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="13" t="s">
-        <v>17</v>
+      <c r="C38" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="20" t="s">
-        <v>23</v>
-      </c>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="21"/>
       <c r="B39" s="3" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="21"/>
-      <c r="B40" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>28</v>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="7"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="9"/>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
-      <c r="G41" s="25"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="18" t="s">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="13"/>
+      <c r="B42" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="6"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B44" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="16" t="s">
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F42" s="17"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="25"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="18"/>
-      <c r="B43" s="4" t="s">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="14"/>
+      <c r="B45" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E43" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F43" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="3">
+      <c r="C45" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
         <v>1</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="3">
+        <v>2</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="3">
+        <v>3</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F44" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="3">
-        <v>2</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D45" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F45" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="3">
-        <v>3</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F46" s="13"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="13">
+      <c r="D48" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="3">
         <v>4</v>
       </c>
-      <c r="B47" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C47" s="13" t="s">
+      <c r="B49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D47" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E47" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F47" s="13"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
+      <c r="D49" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="A51" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>15</v>
+      <c r="A52" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="19"/>
+      <c r="A53" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="B53" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>40</v>
+    <row r="54" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="21"/>
+      <c r="A55" s="12" t="s">
+        <v>17</v>
+      </c>
       <c r="B55" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="10"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="11"/>
+      <c r="A56" s="13"/>
+      <c r="B56" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="14" t="s">
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B57" s="16" t="s">
+      <c r="B58" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C57" s="17"/>
-      <c r="D57" s="18" t="s">
+      <c r="C58" s="18"/>
+      <c r="D58" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E57" s="18"/>
-      <c r="F57" s="1"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="15"/>
-      <c r="B58" s="4" t="s">
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="20"/>
+      <c r="B59" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C58" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F58" s="1"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="3">
-        <v>1</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F59" s="1"/>
+      <c r="C59" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E59" s="1"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>16</v>
+        <v>27</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E60" s="3"/>
-      <c r="F60" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="E60" s="1"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E61" s="3"/>
-      <c r="F61" s="1"/>
+        <v>31</v>
+      </c>
+      <c r="E61" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="17">
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B44:D44"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A52:A53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>